<commit_message>
adding a few scripted things
</commit_message>
<xml_diff>
--- a/data/Type_I_abundance_no_atypicals.xlsx
+++ b/data/Type_I_abundance_no_atypicals.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/dev/kinometree/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Work/Papers/kinome/kinometree/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F195058E-34D8-BA48-BA99-633FAFACFC89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5065D900-2049-AD4B-86E2-9C2B31DE6657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19920" yWindow="1540" windowWidth="22980" windowHeight="26800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="460" windowWidth="22980" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
     <sheet name="Frequencies" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="128">
   <si>
     <t>KLIFS position</t>
   </si>
@@ -320,6 +325,96 @@
   </si>
   <si>
     <t>Proximity_backbone</t>
+  </si>
+  <si>
+    <t>5dls</t>
+  </si>
+  <si>
+    <t>L15</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>very dependent on the conformation</t>
+  </si>
+  <si>
+    <t>V23</t>
+  </si>
+  <si>
+    <t>A36</t>
+  </si>
+  <si>
+    <t>K38</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>E55</t>
+  </si>
+  <si>
+    <t>a bit far away for type I no?</t>
+  </si>
+  <si>
+    <t>N59</t>
+  </si>
+  <si>
+    <t>V68</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>L84</t>
+  </si>
+  <si>
+    <t>F83</t>
+  </si>
+  <si>
+    <t>E85</t>
+  </si>
+  <si>
+    <t>Y86</t>
+  </si>
+  <si>
+    <t>C87</t>
+  </si>
+  <si>
+    <t>I don't understand the sidechain interactions -&gt; examples of structures here?</t>
+  </si>
+  <si>
+    <t>same, rather not directly in contact with sidechain</t>
+  </si>
+  <si>
+    <t>S88</t>
+  </si>
+  <si>
+    <t>same, example where the sidechain is in contact?</t>
   </si>
 </sst>
 </file>
@@ -790,9 +885,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -803,7 +900,7 @@
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="160" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="160" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -834,8 +931,14 @@
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -860,8 +963,11 @@
         <v>20</v>
       </c>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -888,8 +994,11 @@
         <v>6</v>
       </c>
       <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -914,8 +1023,14 @@
       <c r="J4" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -938,8 +1053,11 @@
       <c r="J5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -966,8 +1084,11 @@
       <c r="J6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -988,8 +1109,11 @@
         <v>735</v>
       </c>
       <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -1016,8 +1140,11 @@
         <v>290</v>
       </c>
       <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -1044,8 +1171,14 @@
         <v>185</v>
       </c>
       <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>110</v>
+      </c>
+      <c r="L9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -1072,8 +1205,11 @@
       <c r="J10" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1098,8 +1234,11 @@
         <v>166</v>
       </c>
       <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
@@ -1122,8 +1261,14 @@
         <v>1516</v>
       </c>
       <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -1148,8 +1293,11 @@
         <v>103</v>
       </c>
       <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1176,8 +1324,11 @@
         <v>23</v>
       </c>
       <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -1200,8 +1351,11 @@
         <v>65</v>
       </c>
       <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
@@ -1224,8 +1378,14 @@
       <c r="J16" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" t="s">
+        <v>104</v>
+      </c>
+      <c r="L16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
@@ -1246,8 +1406,11 @@
         <v>97</v>
       </c>
       <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
@@ -1272,8 +1435,14 @@
         <v>318</v>
       </c>
       <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" t="s">
+        <v>105</v>
+      </c>
+      <c r="L18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
@@ -1298,8 +1467,11 @@
       <c r="J19" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
@@ -1320,8 +1492,11 @@
         <v>15</v>
       </c>
       <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -1348,8 +1523,11 @@
         <v>38</v>
       </c>
       <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
@@ -1375,7 +1553,7 @@
       </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
@@ -1403,7 +1581,7 @@
       </c>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>30</v>
       </c>
@@ -1430,8 +1608,11 @@
         <v>16</v>
       </c>
       <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
@@ -1458,8 +1639,14 @@
         <v>29</v>
       </c>
       <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" t="s">
+        <v>114</v>
+      </c>
+      <c r="L25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
@@ -1484,8 +1671,11 @@
         <v>38</v>
       </c>
       <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>33</v>
       </c>
@@ -1511,7 +1701,7 @@
       </c>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>34</v>
       </c>
@@ -1534,8 +1724,11 @@
         <v>15</v>
       </c>
       <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>35</v>
       </c>
@@ -1560,8 +1753,14 @@
         <v>18</v>
       </c>
       <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" t="s">
+        <v>116</v>
+      </c>
+      <c r="L29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>36</v>
       </c>
@@ -1586,8 +1785,11 @@
         <v>16</v>
       </c>
       <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>37</v>
       </c>
@@ -1611,7 +1813,7 @@
       </c>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>38</v>
       </c>
@@ -1637,7 +1839,7 @@
       </c>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>39</v>
       </c>
@@ -1661,7 +1863,7 @@
       </c>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>40</v>
       </c>
@@ -1687,7 +1889,7 @@
       </c>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>41</v>
       </c>
@@ -1715,7 +1917,7 @@
       </c>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>42</v>
       </c>
@@ -1736,8 +1938,11 @@
         <v>13</v>
       </c>
       <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>43</v>
       </c>
@@ -1760,8 +1965,14 @@
         <v>40</v>
       </c>
       <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" t="s">
+        <v>117</v>
+      </c>
+      <c r="L37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>44</v>
       </c>
@@ -1786,8 +1997,11 @@
         <v>163</v>
       </c>
       <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>45</v>
       </c>
@@ -1813,7 +2027,7 @@
       </c>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>46</v>
       </c>
@@ -1841,7 +2055,7 @@
       </c>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>47</v>
       </c>
@@ -1869,7 +2083,7 @@
       </c>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>48</v>
       </c>
@@ -1895,7 +2109,7 @@
       </c>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>49</v>
       </c>
@@ -1921,7 +2135,7 @@
       </c>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>50</v>
       </c>
@@ -1947,7 +2161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>51</v>
       </c>
@@ -1970,8 +2184,11 @@
         <v>20</v>
       </c>
       <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>52</v>
       </c>
@@ -1998,8 +2215,14 @@
         <v>2498</v>
       </c>
       <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" t="s">
+        <v>119</v>
+      </c>
+      <c r="L46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>53</v>
       </c>
@@ -2026,8 +2249,14 @@
       <c r="J47" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" t="s">
+        <v>121</v>
+      </c>
+      <c r="L47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>54</v>
       </c>
@@ -2054,8 +2283,14 @@
         <v>60</v>
       </c>
       <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" t="s">
+        <v>122</v>
+      </c>
+      <c r="L48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>55</v>
       </c>
@@ -2082,8 +2317,14 @@
       <c r="J49" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" t="s">
+        <v>123</v>
+      </c>
+      <c r="L49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>56</v>
       </c>
@@ -2112,8 +2353,14 @@
       <c r="J50" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" t="s">
+        <v>126</v>
+      </c>
+      <c r="L50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>57</v>
       </c>
@@ -2139,7 +2386,7 @@
       </c>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>58</v>
       </c>
@@ -2169,7 +2416,7 @@
       </c>
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>59</v>
       </c>
@@ -2197,7 +2444,7 @@
       </c>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>60</v>
       </c>
@@ -2223,7 +2470,7 @@
       </c>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>61</v>
       </c>
@@ -2251,7 +2498,7 @@
       </c>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>62</v>
       </c>
@@ -2281,7 +2528,7 @@
       </c>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>63</v>
       </c>
@@ -2309,7 +2556,7 @@
       </c>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>64</v>
       </c>
@@ -2331,7 +2578,7 @@
       </c>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>65</v>
       </c>
@@ -2357,7 +2604,7 @@
       </c>
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>66</v>
       </c>
@@ -2383,7 +2630,7 @@
       </c>
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>67</v>
       </c>
@@ -2409,7 +2656,7 @@
       </c>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>68</v>
       </c>
@@ -2431,7 +2678,7 @@
       </c>
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>69</v>
       </c>
@@ -2459,7 +2706,7 @@
       </c>
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>70</v>
       </c>

</xml_diff>